<commit_message>
more beta dispersion and output of results
</commit_message>
<xml_diff>
--- a/usvi_betadisper_by_grouping-2025-03-05.xlsx
+++ b/usvi_betadisper_by_grouping-2025-03-05.xlsx
@@ -8,21 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharongrim/projects/apprill/usvi_temporal/usvi_time/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{63C138FE-09D3-2048-8DDA-DA2A8CC4BD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BD80D3-847D-F049-8900-32825F64D4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="760" windowWidth="27240" windowHeight="16240" activeTab="2" xr2:uid="{1799F0E3-1B04-D547-8C71-5C629723D001}"/>
+    <workbookView xWindow="9820" yWindow="1180" windowWidth="27240" windowHeight="16240" activeTab="2" xr2:uid="{1799F0E3-1B04-D547-8C71-5C629723D001}"/>
   </bookViews>
   <sheets>
     <sheet name="usvi_betadisper_metab_by_groupi" sheetId="1" r:id="rId1"/>
     <sheet name="usvi_betadisper_microb_by_group" sheetId="2" r:id="rId2"/>
     <sheet name="usvi_betadisper_summary" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">usvi_betadisper_summary!$I$3:$K$3</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3278" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3332" uniqueCount="200">
   <si>
     <t>grouping</t>
   </si>
@@ -573,14 +589,65 @@
     <t>Median sample dissimilarity distance when using either all samples, site-specific samples, or site- and time-specific groupings of samples.</t>
   </si>
   <si>
-    <t>Mean beta dispersion for samples in each site and sampling time grouping, calculated for three different dissimilarity medians.</t>
+    <t>Median beta dispersion for samples in each site and sampling time grouping, calculated using as baseline three different dissimilarity spatial medians.</t>
+  </si>
+  <si>
+    <t>med_disp</t>
+  </si>
+  <si>
+    <t>Grouping</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Microbiome</t>
+  </si>
+  <si>
+    <t>Metabolome</t>
+  </si>
+  <si>
+    <t>Median dissimilarity distance</t>
+  </si>
+  <si>
+    <t>Median dispersion for each group</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Lameshur Bay</t>
+  </si>
+  <si>
+    <t>Dawn</t>
+  </si>
+  <si>
+    <t>Afternoon</t>
+  </si>
+  <si>
+    <t>Yawzi Reef</t>
+  </si>
+  <si>
+    <t>Tektite Reef</t>
+  </si>
+  <si>
+    <t>Site-specific</t>
+  </si>
+  <si>
+    <t>Site- and time-specific</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -714,6 +781,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1057,8 +1130,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -14050,101 +14125,117 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7C4BFC-DF93-474E-91EE-9C9014DC9B1C}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A2:Y39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="V4" sqref="V4:Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>182</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="V2" t="s">
+        <v>190</v>
+      </c>
+      <c r="X2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>181</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>171</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K3" t="s">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L3" t="s">
         <v>180</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M3" t="s">
+        <v>184</v>
+      </c>
+      <c r="N3" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
+      <c r="O3" t="s">
+        <v>180</v>
+      </c>
+      <c r="P3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>171</v>
+      </c>
+      <c r="S3" t="s">
+        <v>185</v>
+      </c>
+      <c r="T3" t="s">
+        <v>186</v>
+      </c>
+      <c r="U3" t="s">
+        <v>187</v>
+      </c>
+      <c r="V3" t="s">
+        <v>188</v>
+      </c>
+      <c r="W3" t="s">
+        <v>189</v>
+      </c>
+      <c r="X3" t="s">
+        <v>188</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
         <v>0.24410549236975701</v>
-      </c>
-      <c r="C3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3">
-        <v>0.30341647190267601</v>
-      </c>
-      <c r="M3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B4">
-        <v>0.105043671811829</v>
       </c>
       <c r="C4" t="s">
         <v>172</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
@@ -14153,33 +14244,61 @@
         <v>9</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4">
-        <v>0.30315730637129501</v>
-      </c>
-      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4">
+        <v>0.30341647190267601</v>
+      </c>
+      <c r="P4">
+        <v>0.29846868695428103</v>
+      </c>
+      <c r="Q4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="S4" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V4" s="2">
+        <f>D5</f>
+        <v>0.123859184689553</v>
+      </c>
+      <c r="W4" s="2">
+        <f>B4</f>
+        <v>0.24410549236975701</v>
+      </c>
+      <c r="X4" s="2">
+        <f>M5</f>
+        <v>0.47765062487061399</v>
+      </c>
+      <c r="Y4" s="2">
+        <f>P4</f>
+        <v>0.29846868695428103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5">
-        <v>0.24058624387010799</v>
-      </c>
-      <c r="C5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>0.123859184689553</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>179</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
         <v>9</v>
@@ -14188,30 +14307,49 @@
         <v>22</v>
       </c>
       <c r="L5">
-        <v>0.30818564527693798</v>
-      </c>
-      <c r="M5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.47974279719261598</v>
+      </c>
+      <c r="M5">
+        <v>0.47765062487061399</v>
+      </c>
+      <c r="N5" t="s">
+        <v>179</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2">
+        <f>M7</f>
+        <v>0.478871294824528</v>
+      </c>
+      <c r="Y5" s="2">
+        <f>P6</f>
+        <v>0.299620929616915</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>9.3170086673367195E-2</v>
+        <v>0.13788014309152999</v>
       </c>
       <c r="C6" t="s">
         <v>172</v>
       </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
         <v>9</v>
@@ -14219,174 +14357,297 @@
       <c r="K6" t="s">
         <v>13</v>
       </c>
-      <c r="L6">
-        <v>0.34552591197086102</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="O6">
+        <v>0.30315730637129501</v>
+      </c>
+      <c r="P6">
+        <v>0.299620929616915</v>
+      </c>
+      <c r="Q6" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="T6" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2">
+        <f>M9</f>
+        <v>0.47680717314180499</v>
+      </c>
+      <c r="Y6" s="2">
+        <f>P8</f>
+        <v>0.29338568074633697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>176</v>
-      </c>
-      <c r="B7">
-        <v>0.13367419104942099</v>
-      </c>
-      <c r="C7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>0.106490860213515</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>179</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
         <v>9</v>
       </c>
       <c r="K7" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L7">
-        <v>0.34581732947073501</v>
-      </c>
-      <c r="M7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.48700924468725898</v>
+      </c>
+      <c r="M7">
+        <v>0.478871294824528</v>
+      </c>
+      <c r="N7" t="s">
+        <v>179</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2">
+        <f>M11</f>
+        <v>0.47414125214275399</v>
+      </c>
+      <c r="Y7" s="2">
+        <f>P10</f>
+        <v>0.34368350231677203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B8">
-        <v>0.22185582134384599</v>
+        <v>0.105043671811829</v>
       </c>
       <c r="C8" t="s">
         <v>172</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
         <v>9</v>
       </c>
       <c r="K8" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8">
-        <v>0.336481336465634</v>
-      </c>
-      <c r="M8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8">
+        <v>0.30818564527693798</v>
+      </c>
+      <c r="P8">
+        <v>0.29338568074633697</v>
+      </c>
+      <c r="Q8" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="T8" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2">
+        <f>M13</f>
+        <v>0.47503340594473298</v>
+      </c>
+      <c r="Y8" s="2">
+        <f>P12</f>
+        <v>0.323123655458114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>178</v>
-      </c>
-      <c r="B9">
-        <v>0.240867492321472</v>
-      </c>
-      <c r="C9" t="s">
-        <v>172</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
+        <v>173</v>
+      </c>
+      <c r="D9">
+        <v>8.6123425605180007E-2</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>179</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
       </c>
       <c r="I9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K9" t="s">
         <v>22</v>
       </c>
       <c r="L9">
-        <v>0.102504681253052</v>
-      </c>
-      <c r="M9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.47863606381343299</v>
+      </c>
+      <c r="M9">
+        <v>0.47680717314180499</v>
+      </c>
+      <c r="N9" t="s">
+        <v>179</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2">
+        <f>M15</f>
+        <v>0.47617511741929702</v>
+      </c>
+      <c r="Y9" s="2">
+        <f>P14</f>
+        <v>0.33020338012296102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>176</v>
       </c>
       <c r="B10">
-        <v>0.13788014309152999</v>
+        <v>0.13367419104942099</v>
       </c>
       <c r="C10" t="s">
         <v>172</v>
       </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K10" t="s">
         <v>13</v>
       </c>
-      <c r="L10">
-        <v>0.106392180936476</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="O10">
+        <v>0.34552591197086102</v>
+      </c>
+      <c r="P10">
+        <v>0.34368350231677203</v>
+      </c>
+      <c r="Q10" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="S10" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V10" s="2">
+        <f>D7</f>
+        <v>0.106490860213515</v>
+      </c>
+      <c r="W10" s="2">
+        <f>B8</f>
+        <v>0.105043671811829</v>
+      </c>
+      <c r="X10" s="2">
+        <f>M17</f>
+        <v>0.21080437229371901</v>
+      </c>
+      <c r="Y10" s="2">
+        <f>P16</f>
+        <v>8.8839430572786093E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11">
-        <v>0.24285447039286601</v>
-      </c>
-      <c r="C11" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
+        <v>176</v>
+      </c>
+      <c r="D11">
+        <v>0.16065860968773599</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>179</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
       </c>
       <c r="I11" t="s">
         <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K11" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L11">
-        <v>0.16178679815328301</v>
-      </c>
-      <c r="M11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.475301108362566</v>
+      </c>
+      <c r="M11">
+        <v>0.47414125214275399</v>
+      </c>
+      <c r="N11" t="s">
+        <v>179</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2">
+        <f>M19</f>
+        <v>0.21863811369806899</v>
+      </c>
+      <c r="Y11" s="2">
+        <f>P18</f>
+        <v>0.10029816315746901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -14396,521 +14657,810 @@
       <c r="C12" t="s">
         <v>172</v>
       </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
         <v>9</v>
       </c>
       <c r="I12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K12" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12">
-        <v>0.223792307964712</v>
-      </c>
-      <c r="M12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12">
+        <v>0.34581732947073501</v>
+      </c>
+      <c r="P12">
+        <v>0.323123655458114</v>
+      </c>
+      <c r="Q12" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="T12" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V12" s="2">
+        <f>D13</f>
+        <v>4.2208497668664101E-2</v>
+      </c>
+      <c r="W12" s="2">
+        <f>B14</f>
+        <v>9.3170086673367195E-2</v>
+      </c>
+      <c r="X12" s="2">
+        <f>M21</f>
+        <v>0.200934008009022</v>
+      </c>
+      <c r="Y12" s="2">
+        <f>P20</f>
+        <v>0.13894708478074</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>0.123859184689553</v>
-      </c>
-      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>4.2208497668664101E-2</v>
+      </c>
+      <c r="E13" t="s">
         <v>179</v>
       </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
         <v>9</v>
       </c>
       <c r="I13" t="s">
         <v>23</v>
       </c>
       <c r="J13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K13" t="s">
         <v>22</v>
       </c>
       <c r="L13">
-        <v>0.25377256756985</v>
-      </c>
-      <c r="M13" t="s">
+        <v>0.47845994591353302</v>
+      </c>
+      <c r="M13">
+        <v>0.47503340594473298</v>
+      </c>
+      <c r="N13" t="s">
+        <v>179</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2">
+        <f>M23</f>
+        <v>0.19440470586038699</v>
+      </c>
+      <c r="Y13" s="2">
+        <f>P22</f>
+        <v>0.22697365606188599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14">
+        <v>9.3170086673367195E-2</v>
+      </c>
+      <c r="C14" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>173</v>
-      </c>
-      <c r="B14">
-        <v>8.6123425605180007E-2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>179</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
         <v>22</v>
       </c>
       <c r="I14" t="s">
         <v>23</v>
       </c>
       <c r="J14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K14" t="s">
         <v>13</v>
       </c>
-      <c r="L14">
-        <v>0.24266427348012601</v>
-      </c>
-      <c r="M14" t="s">
+      <c r="O14">
+        <v>0.336481336465634</v>
+      </c>
+      <c r="P14">
+        <v>0.33020338012296102</v>
+      </c>
+      <c r="Q14" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="T14" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V14" s="2">
+        <f>D19</f>
+        <v>5.2928596426127301E-2</v>
+      </c>
+      <c r="W14" s="2">
+        <f>B18</f>
+        <v>0.24285447039286601</v>
+      </c>
+      <c r="X14" s="2">
+        <f>M25</f>
+        <v>0.19144465803596999</v>
+      </c>
+      <c r="Y14" s="2">
+        <f>P24</f>
+        <v>0.22256314074158201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>175</v>
       </c>
-      <c r="B15">
+      <c r="D15">
         <v>4.5337957224635198E-2</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>179</v>
       </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
         <v>22</v>
       </c>
       <c r="I15" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="J15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15">
+        <v>0.48030542765325601</v>
+      </c>
+      <c r="M15">
+        <v>0.47617511741929702</v>
+      </c>
+      <c r="N15" t="s">
+        <v>179</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2">
+        <f>M27</f>
+        <v>0.19466069654350401</v>
+      </c>
+      <c r="Y15" s="2">
+        <f>P26</f>
+        <v>0.23514651067185399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16">
+        <v>0.240867492321472</v>
+      </c>
+      <c r="C16" t="s">
+        <v>172</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16">
+        <v>0.102504681253052</v>
+      </c>
+      <c r="P16">
+        <v>8.8839430572786093E-2</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>172</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V16" s="2">
+        <f>D9</f>
+        <v>8.6123425605180007E-2</v>
+      </c>
+      <c r="W16" s="2">
+        <f>B8</f>
+        <v>0.105043671811829</v>
+      </c>
+      <c r="X16" s="2">
+        <f>M29</f>
+        <v>0.105805341289397</v>
+      </c>
+      <c r="Y16" s="2">
+        <f>P28</f>
+        <v>7.8551195368407503E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17">
+        <v>3.2167354624233799E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17">
+        <v>0.21520231964738801</v>
+      </c>
+      <c r="M17">
+        <v>0.21080437229371901</v>
+      </c>
+      <c r="N17" t="s">
+        <v>179</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V17" s="2">
+        <f>D11</f>
+        <v>0.16065860968773599</v>
+      </c>
+      <c r="W17" s="2">
+        <f>B10</f>
+        <v>0.13367419104942099</v>
+      </c>
+      <c r="X17" s="2">
+        <f>M31</f>
+        <v>0.17873015336044501</v>
+      </c>
+      <c r="Y17" s="2">
+        <f>P30</f>
+        <v>9.0550836735480394E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>0.24285447039286601</v>
+      </c>
+      <c r="C18" t="s">
+        <v>172</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O18">
+        <v>0.106392180936476</v>
+      </c>
+      <c r="P18">
+        <v>0.10029816315746901</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>172</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V18" s="2">
+        <f>D15</f>
+        <v>4.5337957224635198E-2</v>
+      </c>
+      <c r="W18" s="2">
+        <f>B14</f>
+        <v>9.3170086673367195E-2</v>
+      </c>
+      <c r="X18" s="2">
+        <f>M33</f>
+        <v>0.13596971534008201</v>
+      </c>
+      <c r="Y18" s="2">
+        <f>P32</f>
+        <v>7.7150845438203206E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <v>5.2928596426127301E-2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K19" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19">
+        <v>0.23323141858906599</v>
+      </c>
+      <c r="M19">
+        <v>0.21863811369806899</v>
+      </c>
+      <c r="N19" t="s">
+        <v>179</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V19" s="2">
+        <f>D17</f>
+        <v>3.2167354624233799E-2</v>
+      </c>
+      <c r="W19" s="2">
+        <f>B16</f>
+        <v>0.240867492321472</v>
+      </c>
+      <c r="X19" s="2">
+        <f>M35</f>
+        <v>9.0910947066235301E-2</v>
+      </c>
+      <c r="Y19" s="2">
+        <f>P34</f>
+        <v>0.22272243317356399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20">
+        <v>0.24058624387010799</v>
+      </c>
+      <c r="C20" t="s">
+        <v>172</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20">
+        <v>0.16178679815328301</v>
+      </c>
+      <c r="P20">
+        <v>0.13894708478074</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>172</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="V20" s="2">
+        <f>D21</f>
+        <v>4.9077327692110699E-2</v>
+      </c>
+      <c r="W20" s="2">
+        <f>B20</f>
+        <v>0.24058624387010799</v>
+      </c>
+      <c r="X20" s="2">
+        <f>M37</f>
+        <v>9.24680867470761E-2</v>
+      </c>
+      <c r="Y20" s="2">
+        <f>P36</f>
+        <v>0.166376413415151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>174</v>
+      </c>
+      <c r="D21">
+        <v>4.9077327692110699E-2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>179</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21">
+        <v>0.20444039309501999</v>
+      </c>
+      <c r="M21">
+        <v>0.200934008009022</v>
+      </c>
+      <c r="N21" t="s">
+        <v>179</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V21" s="2">
+        <f>D23</f>
+        <v>6.4626920408059493E-2</v>
+      </c>
+      <c r="W21" s="2">
+        <f>B22</f>
+        <v>0.22185582134384599</v>
+      </c>
+      <c r="X21" s="2">
+        <f>M39</f>
+        <v>0.15395587228692201</v>
+      </c>
+      <c r="Y21" s="2">
+        <f>P38</f>
+        <v>0.19812020360454499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>177</v>
+      </c>
+      <c r="B22">
+        <v>0.22185582134384599</v>
+      </c>
+      <c r="C22" t="s">
+        <v>172</v>
+      </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" t="s">
+        <v>13</v>
+      </c>
+      <c r="O22">
+        <v>0.223792307964712</v>
+      </c>
+      <c r="P22">
+        <v>0.22697365606188599</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>177</v>
+      </c>
+      <c r="D23">
+        <v>6.4626920408059493E-2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>179</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23">
+        <v>0.19705621449286401</v>
+      </c>
+      <c r="M23">
+        <v>0.19440470586038699</v>
+      </c>
+      <c r="N23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" t="s">
+        <v>22</v>
+      </c>
+      <c r="O24">
+        <v>0.25377256756985</v>
+      </c>
+      <c r="P24">
+        <v>0.22256314074158201</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25">
+        <v>0.198521655287792</v>
+      </c>
+      <c r="M25">
+        <v>0.19144465803596999</v>
+      </c>
+      <c r="N25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" t="s">
+        <v>13</v>
+      </c>
+      <c r="O26">
+        <v>0.24266427348012601</v>
+      </c>
+      <c r="P26">
+        <v>0.23514651067185399</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I27" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" t="s">
+        <v>8</v>
+      </c>
+      <c r="K27" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27">
+        <v>0.202876124449377</v>
+      </c>
+      <c r="M27">
+        <v>0.19466069654350401</v>
+      </c>
+      <c r="N27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" t="s">
         <v>164</v>
       </c>
-      <c r="K15" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15">
+      <c r="K28" t="s">
+        <v>22</v>
+      </c>
+      <c r="O28">
         <v>9.3129752403343702E-2</v>
       </c>
-      <c r="M15" t="s">
+      <c r="P28">
+        <v>7.8551195368407503E-2</v>
+      </c>
+      <c r="Q28" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>174</v>
-      </c>
-      <c r="B16">
-        <v>4.9077327692110699E-2</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" t="s">
+        <v>164</v>
+      </c>
+      <c r="K29" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29">
+        <v>0.113450052494599</v>
+      </c>
+      <c r="M29">
+        <v>0.105805341289397</v>
+      </c>
+      <c r="N29" t="s">
         <v>179</v>
       </c>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" t="s">
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" t="s">
         <v>164</v>
       </c>
-      <c r="K16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L16">
+      <c r="K30" t="s">
+        <v>13</v>
+      </c>
+      <c r="O30">
         <v>9.4130322129222899E-2</v>
       </c>
-      <c r="M16" t="s">
+      <c r="P30">
+        <v>9.0550836735480394E-2</v>
+      </c>
+      <c r="Q30" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>176</v>
-      </c>
-      <c r="B17">
-        <v>0.16065860968773599</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I31" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" t="s">
+        <v>164</v>
+      </c>
+      <c r="K31" t="s">
+        <v>13</v>
+      </c>
+      <c r="L31">
+        <v>0.19468967628287101</v>
+      </c>
+      <c r="M31">
+        <v>0.17873015336044501</v>
+      </c>
+      <c r="N31" t="s">
         <v>179</v>
       </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" t="s">
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" t="s">
         <v>164</v>
       </c>
-      <c r="K17" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17">
+      <c r="K32" t="s">
+        <v>22</v>
+      </c>
+      <c r="O32">
         <v>0.10283341947793</v>
       </c>
-      <c r="M17" t="s">
+      <c r="P32">
+        <v>7.7150845438203206E-2</v>
+      </c>
+      <c r="Q32" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>178</v>
-      </c>
-      <c r="B18">
-        <v>3.2167354624233799E-2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>179</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K18" t="s">
-        <v>13</v>
-      </c>
-      <c r="L18">
-        <v>0.21902013876465101</v>
-      </c>
-      <c r="M18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>177</v>
-      </c>
-      <c r="B19">
-        <v>6.4626920408059493E-2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>179</v>
-      </c>
-      <c r="D19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" t="s">
-        <v>164</v>
-      </c>
-      <c r="K19" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19">
-        <v>0.204182890359181</v>
-      </c>
-      <c r="M19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20">
-        <v>0.106490860213515</v>
-      </c>
-      <c r="C20" t="s">
-        <v>179</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" t="s">
-        <v>164</v>
-      </c>
-      <c r="K20" t="s">
-        <v>13</v>
-      </c>
-      <c r="L20">
-        <v>0.208939630271509</v>
-      </c>
-      <c r="M20" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>4.2208497668664101E-2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>179</v>
-      </c>
-      <c r="D21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" t="s">
-        <v>9</v>
-      </c>
-      <c r="K21" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21">
-        <v>0.47974279719261598</v>
-      </c>
-      <c r="M21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22">
-        <v>5.2928596426127301E-2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>179</v>
-      </c>
-      <c r="D22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I22" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" t="s">
-        <v>9</v>
-      </c>
-      <c r="K22" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22">
-        <v>0.48700924468725898</v>
-      </c>
-      <c r="M22" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I23" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" t="s">
-        <v>9</v>
-      </c>
-      <c r="K23" t="s">
-        <v>22</v>
-      </c>
-      <c r="L23">
-        <v>0.47845994591353302</v>
-      </c>
-      <c r="M23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" t="s">
-        <v>9</v>
-      </c>
-      <c r="K24" t="s">
-        <v>13</v>
-      </c>
-      <c r="L24">
-        <v>0.48030542765325601</v>
-      </c>
-      <c r="M24" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I25" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" t="s">
-        <v>9</v>
-      </c>
-      <c r="K25" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25">
-        <v>0.47863606381343299</v>
-      </c>
-      <c r="M25" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I26" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" t="s">
-        <v>9</v>
-      </c>
-      <c r="K26" t="s">
-        <v>13</v>
-      </c>
-      <c r="L26">
-        <v>0.475301108362566</v>
-      </c>
-      <c r="M26" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I27" t="s">
-        <v>15</v>
-      </c>
-      <c r="J27" t="s">
-        <v>8</v>
-      </c>
-      <c r="K27" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27">
-        <v>0.21520231964738801</v>
-      </c>
-      <c r="M27" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I28" t="s">
-        <v>15</v>
-      </c>
-      <c r="J28" t="s">
-        <v>8</v>
-      </c>
-      <c r="K28" t="s">
-        <v>13</v>
-      </c>
-      <c r="L28">
-        <v>0.23323141858906599</v>
-      </c>
-      <c r="M28" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I29" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" t="s">
-        <v>8</v>
-      </c>
-      <c r="K29" t="s">
-        <v>22</v>
-      </c>
-      <c r="L29">
-        <v>0.198521655287792</v>
-      </c>
-      <c r="M29" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I30" t="s">
-        <v>23</v>
-      </c>
-      <c r="J30" t="s">
-        <v>8</v>
-      </c>
-      <c r="K30" t="s">
-        <v>13</v>
-      </c>
-      <c r="L30">
-        <v>0.202876124449377</v>
-      </c>
-      <c r="M30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I31" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" t="s">
-        <v>8</v>
-      </c>
-      <c r="K31" t="s">
-        <v>22</v>
-      </c>
-      <c r="L31">
-        <v>0.20444039309501999</v>
-      </c>
-      <c r="M31" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I32" t="s">
-        <v>19</v>
-      </c>
-      <c r="J32" t="s">
-        <v>8</v>
-      </c>
-      <c r="K32" t="s">
-        <v>13</v>
-      </c>
-      <c r="L32">
-        <v>0.19705621449286401</v>
-      </c>
-      <c r="M32" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="33" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="9:17" x14ac:dyDescent="0.2">
       <c r="I33" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J33" t="s">
         <v>164</v>
@@ -14919,15 +15469,18 @@
         <v>22</v>
       </c>
       <c r="L33">
-        <v>0.113450052494599</v>
-      </c>
-      <c r="M33" t="s">
+        <v>0.139947439716578</v>
+      </c>
+      <c r="M33">
+        <v>0.13596971534008201</v>
+      </c>
+      <c r="N33" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="9:17" x14ac:dyDescent="0.2">
       <c r="I34" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J34" t="s">
         <v>164</v>
@@ -14935,31 +15488,37 @@
       <c r="K34" t="s">
         <v>13</v>
       </c>
-      <c r="L34">
-        <v>0.19468967628287101</v>
-      </c>
-      <c r="M34" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="35" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="O34">
+        <v>0.21902013876465101</v>
+      </c>
+      <c r="P34">
+        <v>0.22272243317356399</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="9:17" x14ac:dyDescent="0.2">
       <c r="I35" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J35" t="s">
         <v>164</v>
       </c>
       <c r="K35" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L35">
-        <v>0.102361258147247</v>
-      </c>
-      <c r="M35" t="s">
+        <v>9.5544057784924599E-2</v>
+      </c>
+      <c r="M35">
+        <v>9.0910947066235301E-2</v>
+      </c>
+      <c r="N35" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="9:17" x14ac:dyDescent="0.2">
       <c r="I36" t="s">
         <v>23</v>
       </c>
@@ -14967,18 +15526,21 @@
         <v>164</v>
       </c>
       <c r="K36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L36">
-        <v>0.163014186603989</v>
-      </c>
-      <c r="M36" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="37" spans="9:13" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="O36">
+        <v>0.204182890359181</v>
+      </c>
+      <c r="P36">
+        <v>0.166376413415151</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="9:17" x14ac:dyDescent="0.2">
       <c r="I37" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J37" t="s">
         <v>164</v>
@@ -14987,15 +15549,18 @@
         <v>22</v>
       </c>
       <c r="L37">
-        <v>0.139947439716578</v>
-      </c>
-      <c r="M37" t="s">
+        <v>0.102361258147247</v>
+      </c>
+      <c r="M37">
+        <v>9.24680867470761E-2</v>
+      </c>
+      <c r="N37" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="9:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="9:17" x14ac:dyDescent="0.2">
       <c r="I38" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J38" t="s">
         <v>164</v>
@@ -15003,14 +15568,44 @@
       <c r="K38" t="s">
         <v>13</v>
       </c>
-      <c r="L38">
-        <v>9.5544057784924599E-2</v>
-      </c>
-      <c r="M38" t="s">
+      <c r="O38">
+        <v>0.208939630271509</v>
+      </c>
+      <c r="P38">
+        <v>0.19812020360454499</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="9:17" x14ac:dyDescent="0.2">
+      <c r="I39" t="s">
+        <v>23</v>
+      </c>
+      <c r="J39" t="s">
+        <v>164</v>
+      </c>
+      <c r="K39" t="s">
+        <v>13</v>
+      </c>
+      <c r="L39">
+        <v>0.163014186603989</v>
+      </c>
+      <c r="M39">
+        <v>0.15395587228692201</v>
+      </c>
+      <c r="N39" t="s">
         <v>179</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="I3:N3" xr:uid="{DE7C4BFC-DF93-474E-91EE-9C9014DC9B1C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I4:N35">
+    <sortCondition ref="J4:J35"/>
+    <sortCondition ref="I4:I35"/>
+    <sortCondition ref="K4:K35"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>